<commit_message>
layering utils added, doc update
</commit_message>
<xml_diff>
--- a/doc/Anforderungskatalog.xlsx
+++ b/doc/Anforderungskatalog.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="15360" windowHeight="7500" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="15360" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="Vision" sheetId="5" r:id="rId1"/>
-    <sheet name="Scope" sheetId="6" r:id="rId2"/>
+    <sheet name="Systemkontext" sheetId="8" r:id="rId2"/>
     <sheet name="Ziele" sheetId="1" r:id="rId3"/>
-    <sheet name="Anforderungen" sheetId="2" r:id="rId4"/>
-    <sheet name="AnforderungenDetail" sheetId="7" r:id="rId5"/>
+    <sheet name="Scope" sheetId="6" r:id="rId4"/>
+    <sheet name="Anforderungen" sheetId="2" r:id="rId5"/>
+    <sheet name="AnforderungenDetail" sheetId="7" r:id="rId6"/>
+    <sheet name="References" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -559,7 +561,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="147">
   <si>
     <t>Nummer</t>
   </si>
@@ -777,15 +779,6 @@
     <t>Weltdaten müssen nicht manuell erstellt werden</t>
   </si>
   <si>
-    <t>Mögliche Schwachstellen in einem Verkehrsnetz erkennen.</t>
-  </si>
-  <si>
-    <t>Statistische Daten anhand einer Simulation über ein bestimmtes Verkehrsszenario erheben.</t>
-  </si>
-  <si>
-    <t>Simulation realer Verkehrsnetze.</t>
-  </si>
-  <si>
     <t>1, 2, 3</t>
   </si>
   <si>
@@ -804,12 +797,6 @@
     <t>Vision</t>
   </si>
   <si>
-    <t>Agent-basierte Mikrosimulation auf realen Verkehrsnetzen für den einfachen User ermöglichen.</t>
-  </si>
-  <si>
-    <t>Verschiedene Fahrertypen können simuliert werden.</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -819,12 +806,6 @@
     <t>References</t>
   </si>
   <si>
-    <t>[1] : http://sumo.dlr.de/wiki/Networks/Import/OpenStreetMap</t>
-  </si>
-  <si>
-    <t>[2] : http://sumo.dlr.de/wiki/NETCONVERT</t>
-  </si>
-  <si>
     <t>Visualisierung zweckmässig, nicht Hauptfokus der Arbeit.</t>
   </si>
   <si>
@@ -952,13 +933,82 @@
   </si>
   <si>
     <t>Die KI soll Entscheide treffen  können die das Verhalten des Agents beeinflussen.</t>
+  </si>
+  <si>
+    <t>Systemkontext</t>
+  </si>
+  <si>
+    <t>Ziels ist, dass nach Beendigung des Projekts von einem Anwender Statistische Daten über den Verkehrsfluss pro Zeit über ein bestimmtes Verkehrsszenario erhoben werden können.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ziels ist, dass nach Beendingung des Projekts von einem Anwender Stauherde erkannt werden können. </t>
+  </si>
+  <si>
+    <t>Ziels ist, dass nach Beendidung des Projekts von einem Programmierer flexibel neue Verhaltensmuster für Fahrertypen eingeführt werden können.</t>
+  </si>
+  <si>
+    <t>Hauptziel</t>
+  </si>
+  <si>
+    <t>Unterziel</t>
+  </si>
+  <si>
+    <t>Unterziels ist, dass dem Anwender die jeweiligen Simulationszustaände in einem GUI visualisiert wird.</t>
+  </si>
+  <si>
+    <t>Unterziel ist, dass dem Anwender Informationen zu Geschwindigkeit der Fahrzeuge über das GUI präsentiert wird.</t>
+  </si>
+  <si>
+    <t>Unterziel ist, dass der Anwender über das GUI Verkehrszenarien definieren kann.</t>
+  </si>
+  <si>
+    <t>Unterziel ist, dass der Anwender über das GUI Messpunkte setzen und konfigurieren kann.</t>
+  </si>
+  <si>
+    <t>Unterziel ist, dass der Anwender über das GUI Daten zu den Messpunkten auslesen kann.</t>
+  </si>
+  <si>
+    <t>Ziels ist, dass nach Beendidung des Projekts von einem Anwender reale Strassennetze mit hilfe eines Konvertors [2] von OpenStreetMap importiert werden köennen.</t>
+  </si>
+  <si>
+    <t>Unterziel ist, dass dem Anwender der Konvertor [2] zur verfügung gestellt wird.</t>
+  </si>
+  <si>
+    <t>Unterziel ist, dass der Anwender über das GUI Strassennetze importieren kann.</t>
+  </si>
+  <si>
+    <t>Unterziel ist, dass Programmierer eine Schnittstellt zum Abfragen von situationsspezifischen Simulationsdaten für den Agent zur verfügung steht.</t>
+  </si>
+  <si>
+    <t>Unterziel ist, dass Programmierer eine fest definierte Schnittstellt zum einfügen neuer Verhaltensmuster zur verfügung steht.</t>
+  </si>
+  <si>
+    <t>Unterziel ist, dass Programmierer im GUI neue Verhaltensmuster erfassen können.</t>
+  </si>
+  <si>
+    <t>Der Java Traffic Simulator (JTS) ist eine Agent-basierte Mikrosimulation auf realen Verkehrsnetzen für den ein-fachen User. Das Projekt wird im Rahmen des Modules: Projekt 1 der Berner Fachhochschulen Abteilung Tech-nik und Informatik realisiert.</t>
+  </si>
+  <si>
+    <t>Nr</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <t>http://sumo.dlr.de/wiki/Networks/Import/OpenStreetMap</t>
+  </si>
+  <si>
+    <t>http://sumo.dlr.de/wiki/NETCONVERT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1002,6 +1052,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1041,10 +1099,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1080,8 +1139,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1092,6 +1155,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9010650</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38100" y="876300"/>
+          <a:ext cx="8972550" cy="2505075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1383,28 +1495,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="108.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="226" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1414,10 +1526,190 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="137.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="165.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="13"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1.2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1.3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2.1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>3.1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>3.2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>4.2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>4.3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,12 +1719,12 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>1</v>
@@ -1440,53 +1732,33 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1495,76 +1767,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="93.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,7 +1810,7 @@
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>1</v>
@@ -1684,7 +1892,7 @@
         <v>41907</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1720,7 +1928,7 @@
         <v>41907</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1756,7 +1964,7 @@
         <v>41907</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1792,7 +2000,7 @@
         <v>41907</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1828,7 +2036,7 @@
         <v>41907</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1836,7 +2044,7 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>21</v>
@@ -1864,7 +2072,7 @@
         <v>41907</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1900,7 +2108,7 @@
         <v>41907</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1955,7 +2163,7 @@
         <v>41907</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1991,7 +2199,7 @@
         <v>41907</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -2099,7 +2307,7 @@
         <v>41907</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2135,7 +2343,7 @@
         <v>41907</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2171,7 +2379,7 @@
         <v>41907</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2226,7 +2434,7 @@
         <v>41907</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2234,7 +2442,7 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>21</v>
@@ -2262,7 +2470,7 @@
         <v>41907</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2270,7 +2478,7 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>21</v>
@@ -2325,12 +2533,12 @@
         <v>41907</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C30" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
         <v>48</v>
@@ -2361,12 +2569,12 @@
         <v>41907</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C31" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
         <v>49</v>
@@ -2397,7 +2605,7 @@
         <v>41907</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2433,12 +2641,12 @@
         <v>41907</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D33" t="s">
         <v>56</v>
@@ -2469,7 +2677,7 @@
         <v>41907</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2524,7 +2732,7 @@
         <v>41907</v>
       </c>
       <c r="M37" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2560,7 +2768,7 @@
         <v>41907</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -2615,7 +2823,7 @@
         <v>41907</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -2651,7 +2859,7 @@
         <v>41907</v>
       </c>
       <c r="M43" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2687,7 +2895,7 @@
         <v>41907</v>
       </c>
       <c r="M44" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -2723,7 +2931,7 @@
         <v>41907</v>
       </c>
       <c r="M45" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -2759,7 +2967,7 @@
         <v>41907</v>
       </c>
       <c r="M46" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -2795,7 +3003,7 @@
         <v>41907</v>
       </c>
       <c r="M47" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -2831,7 +3039,7 @@
         <v>41907</v>
       </c>
       <c r="M48" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2854,11 +3062,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -2887,7 +3095,7 @@
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2912,7 +3120,7 @@
       </c>
       <c r="C6" s="7"/>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2922,7 +3130,7 @@
       </c>
       <c r="C7" s="7"/>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2932,7 +3140,7 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2942,7 +3150,7 @@
       </c>
       <c r="C9" s="7"/>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2952,7 +3160,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2962,7 +3170,7 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2972,7 +3180,7 @@
       </c>
       <c r="C12" s="7"/>
       <c r="D12" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3002,7 +3210,7 @@
       </c>
       <c r="C16" s="7"/>
       <c r="D16" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -3012,7 +3220,7 @@
       </c>
       <c r="C17" s="7"/>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -3022,7 +3230,7 @@
       </c>
       <c r="C18" s="7"/>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -3032,7 +3240,7 @@
       </c>
       <c r="C19" s="7"/>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -3052,7 +3260,7 @@
       </c>
       <c r="C21" s="7"/>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -3062,7 +3270,7 @@
       </c>
       <c r="C22" s="7"/>
       <c r="D22" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -3092,7 +3300,7 @@
       </c>
       <c r="C26" s="7"/>
       <c r="D26" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -3102,7 +3310,7 @@
       </c>
       <c r="C27" s="7"/>
       <c r="D27" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E27" s="2"/>
       <c r="G27" s="2"/>
@@ -3119,7 +3327,7 @@
       </c>
       <c r="C28" s="7"/>
       <c r="D28" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="7"/>
@@ -3137,7 +3345,7 @@
       </c>
       <c r="C29" s="7"/>
       <c r="D29" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E29" s="2"/>
       <c r="G29" s="2"/>
@@ -3151,10 +3359,10 @@
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E30" s="2"/>
       <c r="G30" s="2"/>
@@ -3168,10 +3376,10 @@
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E31" s="2"/>
       <c r="G31" s="2"/>
@@ -3188,7 +3396,7 @@
       </c>
       <c r="C32" s="7"/>
       <c r="D32" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E32" s="2"/>
       <c r="G32" s="2"/>
@@ -3201,11 +3409,11 @@
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E33" s="2"/>
       <c r="G33" s="2"/>
@@ -3237,7 +3445,7 @@
       </c>
       <c r="C36" s="7"/>
       <c r="D36" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -3247,7 +3455,7 @@
       </c>
       <c r="C37" s="7"/>
       <c r="D37" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -3276,7 +3484,7 @@
       </c>
       <c r="C41" s="7"/>
       <c r="D41" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E41" s="2"/>
       <c r="G41" s="2"/>
@@ -3293,7 +3501,7 @@
       </c>
       <c r="C42" s="7"/>
       <c r="D42" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E42" s="2"/>
       <c r="G42" s="2"/>
@@ -3310,7 +3518,7 @@
         <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E43" s="2"/>
       <c r="G43" s="2"/>
@@ -3327,7 +3535,7 @@
         <v>67</v>
       </c>
       <c r="D44" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E44" s="2"/>
       <c r="G44" s="2"/>
@@ -3344,7 +3552,7 @@
       </c>
       <c r="C45" s="7"/>
       <c r="D45" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E45" s="2"/>
       <c r="G45" s="2"/>
@@ -3448,4 +3656,56 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>